<commit_message>
new regs, test runs
</commit_message>
<xml_diff>
--- a/cdf_star_by_state.xlsx
+++ b/cdf_star_by_state.xlsx
@@ -404,8 +404,8 @@
   <dimension ref="A1:H190"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E165" sqref="E165:E170"/>
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M55" sqref="M55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>